<commit_message>
Calcolati indici gulpease, stesura resoconto validazione e  collaudo
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiSupporto.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiSupporto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\qualitàProcesso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C214C73-5F28-436A-8F2B-604094DEB7F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B05B4D7-9B7B-4BE7-B852-76A8C285FB71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3440947A-BDC3-41E2-B8C4-C01620109B14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3440947A-BDC3-41E2-B8C4-C01620109B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentazione" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="55">
   <si>
     <t>Indice Gulpease</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Incremento 10</t>
+  </si>
+  <si>
+    <t>3.1.0</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
   </si>
 </sst>
 </file>
@@ -939,10 +945,10 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>75</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,6 +1086,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>75</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5733,9 +5763,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$82:$B$89</c:f>
+              <c:f>Documentazione!$B$82:$B$91</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -5759,16 +5789,22 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$C$82:$C$89</c:f>
+              <c:f>Documentazione!$C$82:$C$91</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>60</c:v>
                 </c:pt>
@@ -5792,6 +5828,12 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5831,9 +5873,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$82:$B$89</c:f>
+              <c:f>Documentazione!$B$82:$B$91</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -5857,16 +5899,22 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$D$82:$D$89</c:f>
+              <c:f>Documentazione!$D$82:$D$91</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -5889,6 +5937,12 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
@@ -5929,9 +5983,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$82:$B$89</c:f>
+              <c:f>Documentazione!$B$82:$B$91</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -5955,16 +6009,22 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$E$82:$E$89</c:f>
+              <c:f>Documentazione!$E$82:$E$91</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
@@ -5987,6 +6047,12 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
@@ -6499,9 +6565,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$105:$B$111</c:f>
+              <c:f>Documentazione!$B$105:$B$113</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -6522,16 +6588,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$C$105:$C$111</c:f>
+              <c:f>Documentazione!$C$105:$C$113</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>70</c:v>
                 </c:pt>
@@ -6552,6 +6624,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6591,9 +6669,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$105:$B$111</c:f>
+              <c:f>Documentazione!$B$105:$B$113</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -6614,16 +6692,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$D$105:$D$111</c:f>
+              <c:f>Documentazione!$D$105:$D$113</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -6643,6 +6727,12 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
@@ -6683,9 +6773,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$105:$B$111</c:f>
+              <c:f>Documentazione!$B$105:$B$113</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -6706,16 +6796,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$E$105:$E$111</c:f>
+              <c:f>Documentazione!$E$105:$E$113</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
@@ -6735,6 +6831,12 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
@@ -7247,9 +7349,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$124:$B$130</c:f>
+              <c:f>Documentazione!$B$124:$B$132</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -7270,16 +7372,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$C$124:$C$130</c:f>
+              <c:f>Documentazione!$C$124:$C$132</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>64</c:v>
                 </c:pt>
@@ -7300,6 +7408,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7339,9 +7453,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$124:$B$130</c:f>
+              <c:f>Documentazione!$B$124:$B$132</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -7362,16 +7476,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$D$124:$D$130</c:f>
+              <c:f>Documentazione!$D$124:$D$132</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -7391,6 +7511,12 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
@@ -7431,9 +7557,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Documentazione!$B$124:$B$130</c:f>
+              <c:f>Documentazione!$B$124:$B$132</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.1.0</c:v>
                 </c:pt>
@@ -7454,16 +7580,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Documentazione!$E$124:$E$130</c:f>
+              <c:f>Documentazione!$E$124:$E$132</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
@@ -7483,6 +7615,12 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
@@ -19026,8 +19164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AECFA2-8686-4F57-8313-C78888B00A1F}">
   <dimension ref="B2:P265"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="C205" sqref="C205:C211"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D178" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19098,7 +19236,9 @@
       <c r="E4" s="2">
         <v>71</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>72</v>
+      </c>
       <c r="G4" s="2">
         <v>40</v>
       </c>
@@ -19119,7 +19259,9 @@
       <c r="E5" s="2">
         <v>71</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <v>75</v>
+      </c>
       <c r="G5" s="2">
         <v>40</v>
       </c>
@@ -19140,7 +19282,9 @@
       <c r="E6" s="2">
         <v>66</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <v>71</v>
+      </c>
       <c r="G6" s="2">
         <v>40</v>
       </c>
@@ -19184,7 +19328,9 @@
       <c r="E8" s="2">
         <v>58</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2">
+        <v>58</v>
+      </c>
       <c r="G8" s="7">
         <v>40</v>
       </c>
@@ -19205,7 +19351,9 @@
       <c r="E9" s="2">
         <v>62</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <v>60</v>
+      </c>
       <c r="G9" s="2">
         <v>40</v>
       </c>
@@ -19226,7 +19374,9 @@
       <c r="E10" s="2">
         <v>60</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2">
+        <v>60</v>
+      </c>
       <c r="G10" s="2">
         <v>40</v>
       </c>
@@ -19241,9 +19391,11 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2">
+        <v>65</v>
+      </c>
+      <c r="F11" s="2">
         <v>72</v>
       </c>
-      <c r="F11" s="2"/>
       <c r="G11" s="2">
         <v>40</v>
       </c>
@@ -19258,9 +19410,11 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2">
+        <v>69</v>
+      </c>
+      <c r="F12" s="2">
         <v>75</v>
       </c>
-      <c r="F12" s="2"/>
       <c r="G12" s="2">
         <v>40</v>
       </c>
@@ -19671,6 +19825,34 @@
         <v>80</v>
       </c>
     </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B90" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C90" s="2">
+        <v>72</v>
+      </c>
+      <c r="D90" s="2">
+        <v>40</v>
+      </c>
+      <c r="E90" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B91" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C91" s="2">
+        <v>72</v>
+      </c>
+      <c r="D91" s="2">
+        <v>40</v>
+      </c>
+      <c r="E91" s="2">
+        <v>80</v>
+      </c>
+    </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103" s="1" t="s">
         <v>19</v>
@@ -19794,6 +19976,34 @@
         <v>80</v>
       </c>
     </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B112" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C112" s="2">
+        <v>73</v>
+      </c>
+      <c r="D112" s="2">
+        <v>40</v>
+      </c>
+      <c r="E112" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B113" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C113" s="2">
+        <v>75</v>
+      </c>
+      <c r="D113" s="2">
+        <v>40</v>
+      </c>
+      <c r="E113" s="2">
+        <v>80</v>
+      </c>
+    </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B122" s="1" t="s">
         <v>20</v>
@@ -19917,6 +20127,34 @@
         <v>80</v>
       </c>
     </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B131" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C131" s="2">
+        <v>65</v>
+      </c>
+      <c r="D131" s="2">
+        <v>40</v>
+      </c>
+      <c r="E131" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B132" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C132" s="2">
+        <v>71</v>
+      </c>
+      <c r="D132" s="2">
+        <v>40</v>
+      </c>
+      <c r="E132" s="2">
+        <v>80</v>
+      </c>
+    </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143" s="1" t="s">
         <v>21</v>
@@ -20104,6 +20342,34 @@
         <v>40</v>
       </c>
       <c r="E173" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B174" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C174" s="2">
+        <v>58</v>
+      </c>
+      <c r="D174" s="2">
+        <v>40</v>
+      </c>
+      <c r="E174" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="175" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B175" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C175" s="2">
+        <v>58</v>
+      </c>
+      <c r="D175" s="2">
+        <v>40</v>
+      </c>
+      <c r="E175" s="2">
         <v>80</v>
       </c>
     </row>
@@ -20353,7 +20619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3418E276-9CB5-4CBF-AFD3-1C3E1A23D165}">
   <dimension ref="C4:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
+    <sheetView topLeftCell="B226" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modify code coverage FE
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiSupporto.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiSupporto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\qualitàProcesso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CCA2AE-8496-47C4-9296-ABFBD85E40DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD55F16-8FBC-4B04-BF77-E769E2669017}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3440947A-BDC3-41E2-B8C4-C01620109B14}"/>
   </bookViews>
@@ -2480,13 +2480,13 @@
                   <c:v>0.81</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.81</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.81</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.81</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20906,8 +20906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3418E276-9CB5-4CBF-AFD3-1C3E1A23D165}">
   <dimension ref="C4:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B226" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21038,7 +21038,7 @@
         <v>55</v>
       </c>
       <c r="D12" s="20">
-        <v>0.81</v>
+        <v>0.83</v>
       </c>
       <c r="E12" s="20">
         <v>0.8</v>
@@ -21052,7 +21052,7 @@
         <v>56</v>
       </c>
       <c r="D13" s="20">
-        <v>0.81</v>
+        <v>0.83</v>
       </c>
       <c r="E13" s="20">
         <v>0.8</v>
@@ -21066,7 +21066,7 @@
         <v>57</v>
       </c>
       <c r="D14" s="20">
-        <v>0.81</v>
+        <v>0.83</v>
       </c>
       <c r="E14" s="20">
         <v>0.8</v>

</xml_diff>